<commit_message>
parser: Grow slice if necessary
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieshuang/gocode/src/github.com/nlimpid/go-xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCA46FC-CB69-A049-AE6B-6BD8F05D36C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87856FD3-D38A-FF40-89DC-3E053418E7FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,6 +451,66 @@
         <v>9.4413881351130304E+17</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
unmarshal: handle tag in struct
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jieshuang/gocode/src/github.com/nlimpid/go-xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87856FD3-D38A-FF40-89DC-3E053418E7FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A208EF-DEA6-5942-B76F-01BF7AB552F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,18 +28,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>order_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>express_company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="9"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -64,10 +86,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -419,96 +442,291 @@
     <col min="2" max="5" width="20" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
-        <v>1056</v>
-      </c>
-      <c r="B1" s="1">
-        <v>22</v>
-      </c>
-      <c r="C1" s="2">
-        <v>43429</v>
-      </c>
-      <c r="D1" s="1">
-        <v>233</v>
-      </c>
-      <c r="E1" s="1">
-        <v>322</v>
-      </c>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>9.4413881351130304E+17</v>
+        <v>1056</v>
+      </c>
+      <c r="B2" s="1">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43429</v>
+      </c>
+      <c r="D2" s="1">
+        <v>233</v>
+      </c>
+      <c r="E2" s="1">
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B3" s="1">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43430</v>
+      </c>
+      <c r="D3" s="1">
+        <v>234</v>
+      </c>
+      <c r="E3" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B4" s="1">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43431</v>
+      </c>
+      <c r="D4" s="1">
+        <v>235</v>
+      </c>
+      <c r="E4" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B5" s="1">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43432</v>
+      </c>
+      <c r="D5" s="1">
+        <v>236</v>
+      </c>
+      <c r="E5" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B6" s="1">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43433</v>
+      </c>
+      <c r="D6" s="1">
+        <v>237</v>
+      </c>
+      <c r="E6" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B7" s="1">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43434</v>
+      </c>
+      <c r="D7" s="1">
+        <v>238</v>
+      </c>
+      <c r="E7" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B8" s="1">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43435</v>
+      </c>
+      <c r="D8" s="1">
+        <v>239</v>
+      </c>
+      <c r="E8" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B9" s="1">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43436</v>
+      </c>
+      <c r="D9" s="1">
+        <v>240</v>
+      </c>
+      <c r="E9" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B10" s="1">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43437</v>
+      </c>
+      <c r="D10" s="1">
+        <v>241</v>
+      </c>
+      <c r="E10" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B11" s="1">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43438</v>
+      </c>
+      <c r="D11" s="1">
+        <v>242</v>
+      </c>
+      <c r="E11" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B12" s="1">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43439</v>
+      </c>
+      <c r="D12" s="1">
+        <v>243</v>
+      </c>
+      <c r="E12" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B13" s="1">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43440</v>
+      </c>
+      <c r="D13" s="1">
+        <v>244</v>
+      </c>
+      <c r="E13" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B14" s="1">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2">
+        <v>43441</v>
+      </c>
+      <c r="D14" s="1">
+        <v>245</v>
+      </c>
+      <c r="E14" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>9.4413881351130304E+17</v>
       </c>
+      <c r="B15" s="1">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43442</v>
+      </c>
+      <c r="D15" s="1">
+        <v>246</v>
+      </c>
+      <c r="E15" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>9.4413881351130304E+17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43443</v>
+      </c>
+      <c r="D16" s="1">
+        <v>247</v>
+      </c>
+      <c r="E16" s="1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>9.4413881351130304E+17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43444</v>
+      </c>
+      <c r="D17" s="1">
+        <v>248</v>
+      </c>
+      <c r="E17" s="1">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>